<commit_message>
fix double precision issue
fix double precision issue
</commit_message>
<xml_diff>
--- a/doc/naive_bayes_sample_excel.xlsx
+++ b/doc/naive_bayes_sample_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Java-Naive-Bayes-Classifier-JNBC\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C828F0-5B4A-480C-A32A-4EE3F6A11858}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832669BD-F5D8-4F1F-9A42-69A4909F5779}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="7" xr2:uid="{5DD707F2-665C-4F54-8809-F4F2A936AEF3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{5DD707F2-665C-4F54-8809-F4F2A936AEF3}"/>
   </bookViews>
   <sheets>
     <sheet name="sample1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="140">
   <si>
     <t xml:space="preserve"> Hot</t>
   </si>
@@ -456,6 +456,12 @@
   </si>
   <si>
     <t>~gL//~fE//X2=L</t>
+  </si>
+  <si>
+    <t>key (path)</t>
+  </si>
+  <si>
+    <t>value (counter)</t>
   </si>
 </sst>
 </file>
@@ -464,9 +470,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,6 +491,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -531,7 +545,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -542,7 +556,8 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -863,8 +878,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{57FC5204-20BF-4133-86B5-A9E318DA254F}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="N21:P25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E93B467-7CD4-4440-BD75-7FDE97455E08}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="R30:S33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
       <items count="4">
@@ -876,14 +891,14 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="3">
         <item x="1"/>
         <item x="0"/>
@@ -893,7 +908,7 @@
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="3"/>
+    <field x="4"/>
   </rowFields>
   <rowItems count="3">
     <i>
@@ -906,19 +921,11 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -933,8 +940,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C81B27A-3948-470C-9D29-F636E72728D4}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="J21:L25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E61A50E0-C108-4B58-A1A8-333579B6799B}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="R21:S24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
       <items count="4">
@@ -945,15 +952,15 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="3">
         <item x="1"/>
         <item x="0"/>
@@ -963,7 +970,7 @@
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="2"/>
+    <field x="4"/>
   </rowFields>
   <rowItems count="3">
     <i>
@@ -976,16 +983,8 @@
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Observation" fld="5" baseField="0" baseItem="0"/>
@@ -1003,6 +1002,73 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9F8D8C1C-3D4B-4E3E-9BB6-631303303054}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B30:D35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8AEAFA69-ED44-492F-954A-EC870EAAC390}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J21:L25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
@@ -1072,7 +1138,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F77E175A-8D61-414C-80B4-55CAF5EF1662}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="R21:S24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
@@ -1134,7 +1200,69 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64F9299C-C3B7-4571-A751-90AFB2CB48A5}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="R30:S33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7377CCE0-6486-4D26-A772-3EC0FA7A1B67}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F30:H35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
@@ -1208,276 +1336,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C191547-023A-4450-B480-D3440E7390E4}" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="J30:L34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{638DB6E6-5B4D-45F7-8A8A-1DAD24D54DB0}" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="N30:P34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9F8D8C1C-3D4B-4E3E-9BB6-631303303054}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B30:D35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64F9299C-C3B7-4571-A751-90AFB2CB48A5}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="R30:S33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D533B6E1-FF8D-4AA1-A7D5-D721D65A2BD8}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B21:D26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
@@ -1544,7 +1403,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2762BB30-B462-461F-B78D-B365DEB0BBE5}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F21:H26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
@@ -1618,9 +1477,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{476D76E7-B827-4379-85D8-AF9D65C273AA}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="F21:H26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7C191547-023A-4450-B480-D3440E7390E4}" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="J30:L34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0">
       <items count="4">
@@ -1630,15 +1489,14 @@
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="4">
+      <items count="3">
         <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisCol" showAll="0">
       <items count="3">
@@ -1650,17 +1508,14 @@
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="1"/>
+    <field x="2"/>
   </rowFields>
-  <rowItems count="4">
+  <rowItems count="3">
     <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
@@ -1678,7 +1533,7 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1692,7 +1547,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2AF659C0-F0C8-4D92-9B90-C6B98663ED3E}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="N21:P25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
@@ -1762,7 +1617,330 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C81B27A-3948-470C-9D29-F636E72728D4}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="J21:L25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{638DB6E6-5B4D-45F7-8A8A-1DAD24D54DB0}" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="N30:P34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7E2F67A-8542-4AF7-8624-9C9125E14C8E}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L21:M24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E22ED947-C6F5-4442-A021-7FCD16A1CEE6}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B31:E36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="3" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6BD64302-94A3-4101-A258-21641D66AF30}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G31:J36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="3" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable24.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6F81060C-D6C8-4D2B-B2C0-241A3F1B9FDB}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G21:J26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
@@ -1830,7 +2008,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable25.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FD7D612-55A4-4052-8A3C-D1DA68AB7A3F}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B21:E26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
@@ -1885,189 +2063,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Observation" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A7E2F67A-8542-4AF7-8624-9C9125E14C8E}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="L21:M24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E22ED947-C6F5-4442-A021-7FCD16A1CEE6}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B31:E36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="3" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6BD64302-94A3-4101-A258-21641D66AF30}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G31:J36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="3" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2333,8 +2328,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62EEF72E-2F3F-4D71-9374-E42B3966A7F7}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B21:D26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB079156-A028-4ACC-B45F-5C20AF7D4A71}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B30:D35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -2385,7 +2380,7 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2468,135 +2463,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E93B467-7CD4-4440-BD75-7FDE97455E08}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="R30:S33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB079156-A028-4ACC-B45F-5C20AF7D4A71}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B30:D35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{73FCD2B1-4D62-4786-A92B-6A771F40503A}" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="N30:P34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
@@ -2653,6 +2519,150 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{57FC5204-20BF-4133-86B5-A9E318DA254F}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="N21:P25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{476D76E7-B827-4379-85D8-AF9D65C273AA}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="F21:H26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -2737,6 +2747,73 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62EEF72E-2F3F-4D71-9374-E42B3966A7F7}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B21:D26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Observation" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DD4D01A5-8B85-4036-BA6F-504E86F4E79C}" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F30:H35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
@@ -2797,68 +2874,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Observation" fld="5" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E61A50E0-C108-4B58-A1A8-333579B6799B}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="R21:S24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Observation" fld="5" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3229,7 +3244,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32:H32"/>
-      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" max="4" activeRow="31" activeCol="5" previousRow="31" previousCol="5" click="1" r:id="rId8">
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" max="4" activeRow="31" activeCol="5" previousRow="31" previousCol="5" click="1" r:id="rId9">
         <pivotArea dataOnly="0" fieldPosition="0">
           <references count="1">
             <reference field="1" count="1">
@@ -4165,21 +4180,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B647E678-FD78-45CC-8F6B-B4C05C2A08A6}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
+      <c r="A1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4427,6 +4443,7 @@
     <sortCondition descending="1" ref="A31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7729,7 +7746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{087EC54C-DD7D-4557-8207-24F8ECC26FA3}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>

</xml_diff>